<commit_message>
Update results with corrected TwelveBarBreakout
- Regenerated all 28 stock analyses
- TwelveBarBreakout now checks previous swing low only

🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/results/AMC.xlsx
+++ b/results/AMC.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P126"/>
+  <dimension ref="A1:P179"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6612,6 +6612,2568 @@
       </c>
       <c r="P126" t="n">
         <v>-5.92654767309057</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="inlineStr">
+        <is>
+          <t>twelve_bar_breakout</t>
+        </is>
+      </c>
+      <c r="B127" t="n">
+        <v>44</v>
+      </c>
+      <c r="C127" t="inlineStr"/>
+      <c r="D127" t="n">
+        <v>0.4026007950305938</v>
+      </c>
+      <c r="E127" t="n">
+        <v>1.623631166712736</v>
+      </c>
+      <c r="F127" t="b">
+        <v>1</v>
+      </c>
+      <c r="G127" t="n">
+        <v>19.64451908502769</v>
+      </c>
+      <c r="H127" t="n">
+        <v>42</v>
+      </c>
+      <c r="I127" t="n">
+        <v>-4.932733567097755</v>
+      </c>
+      <c r="J127" t="n">
+        <v>13</v>
+      </c>
+      <c r="K127" t="b">
+        <v>0</v>
+      </c>
+      <c r="L127" t="inlineStr"/>
+      <c r="M127" t="inlineStr"/>
+      <c r="N127" t="n">
+        <v>18.02088791831495</v>
+      </c>
+      <c r="O127" t="inlineStr"/>
+      <c r="P127" t="inlineStr"/>
+    </row>
+    <row r="128">
+      <c r="A128" t="inlineStr">
+        <is>
+          <t>twelve_bar_breakout</t>
+        </is>
+      </c>
+      <c r="B128" t="n">
+        <v>86</v>
+      </c>
+      <c r="C128" t="inlineStr"/>
+      <c r="D128" t="n">
+        <v>0.4816888570785522</v>
+      </c>
+      <c r="E128" t="n">
+        <v>-13.20562976851282</v>
+      </c>
+      <c r="F128" t="b">
+        <v>0</v>
+      </c>
+      <c r="G128" t="n">
+        <v>0.0001926489031615257</v>
+      </c>
+      <c r="H128" t="n">
+        <v>0</v>
+      </c>
+      <c r="I128" t="n">
+        <v>-17.40874536806627</v>
+      </c>
+      <c r="J128" t="n">
+        <v>27</v>
+      </c>
+      <c r="K128" t="b">
+        <v>1</v>
+      </c>
+      <c r="L128" t="n">
+        <v>27</v>
+      </c>
+      <c r="M128" t="n">
+        <v>-17.40874536806627</v>
+      </c>
+      <c r="N128" t="n">
+        <v>13.20582241741599</v>
+      </c>
+      <c r="O128" t="n">
+        <v>-4.203115599553445</v>
+      </c>
+      <c r="P128" t="n">
+        <v>-17.40893801696943</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="inlineStr">
+        <is>
+          <t>twelve_bar_breakout</t>
+        </is>
+      </c>
+      <c r="B129" t="n">
+        <v>157</v>
+      </c>
+      <c r="C129" t="inlineStr"/>
+      <c r="D129" t="n">
+        <v>0.4460541307926178</v>
+      </c>
+      <c r="E129" t="n">
+        <v>63.05469605888064</v>
+      </c>
+      <c r="F129" t="b">
+        <v>1</v>
+      </c>
+      <c r="G129" t="n">
+        <v>71.83456284115752</v>
+      </c>
+      <c r="H129" t="n">
+        <v>52</v>
+      </c>
+      <c r="I129" t="n">
+        <v>-6.603793207385585</v>
+      </c>
+      <c r="J129" t="n">
+        <v>0</v>
+      </c>
+      <c r="K129" t="b">
+        <v>0</v>
+      </c>
+      <c r="L129" t="inlineStr"/>
+      <c r="M129" t="inlineStr"/>
+      <c r="N129" t="n">
+        <v>8.779866782276876</v>
+      </c>
+      <c r="O129" t="inlineStr"/>
+      <c r="P129" t="inlineStr"/>
+    </row>
+    <row r="130">
+      <c r="A130" t="inlineStr">
+        <is>
+          <t>twelve_bar_breakout</t>
+        </is>
+      </c>
+      <c r="B130" t="n">
+        <v>300</v>
+      </c>
+      <c r="C130" t="inlineStr"/>
+      <c r="D130" t="n">
+        <v>1.21620500087738</v>
+      </c>
+      <c r="E130" t="n">
+        <v>-7.373214208175496</v>
+      </c>
+      <c r="F130" t="b">
+        <v>0</v>
+      </c>
+      <c r="G130" t="n">
+        <v>6.318958325634881</v>
+      </c>
+      <c r="H130" t="n">
+        <v>14</v>
+      </c>
+      <c r="I130" t="n">
+        <v>-7.723164276939428</v>
+      </c>
+      <c r="J130" t="n">
+        <v>0</v>
+      </c>
+      <c r="K130" t="b">
+        <v>0</v>
+      </c>
+      <c r="L130" t="inlineStr"/>
+      <c r="M130" t="inlineStr"/>
+      <c r="N130" t="n">
+        <v>13.69217253381038</v>
+      </c>
+      <c r="O130" t="inlineStr"/>
+      <c r="P130" t="inlineStr"/>
+    </row>
+    <row r="131">
+      <c r="A131" t="inlineStr">
+        <is>
+          <t>twelve_bar_breakout</t>
+        </is>
+      </c>
+      <c r="B131" t="n">
+        <v>374</v>
+      </c>
+      <c r="C131" t="inlineStr"/>
+      <c r="D131" t="n">
+        <v>1.212300539016724</v>
+      </c>
+      <c r="E131" t="n">
+        <v>-7.199685255362234</v>
+      </c>
+      <c r="F131" t="b">
+        <v>0</v>
+      </c>
+      <c r="G131" t="n">
+        <v>15.17094130555305</v>
+      </c>
+      <c r="H131" t="n">
+        <v>18</v>
+      </c>
+      <c r="I131" t="n">
+        <v>-7.199685255362234</v>
+      </c>
+      <c r="J131" t="n">
+        <v>52</v>
+      </c>
+      <c r="K131" t="b">
+        <v>0</v>
+      </c>
+      <c r="L131" t="inlineStr"/>
+      <c r="M131" t="inlineStr"/>
+      <c r="N131" t="n">
+        <v>22.37062656091528</v>
+      </c>
+      <c r="O131" t="inlineStr"/>
+      <c r="P131" t="inlineStr"/>
+    </row>
+    <row r="132">
+      <c r="A132" t="inlineStr">
+        <is>
+          <t>twelve_bar_breakout</t>
+        </is>
+      </c>
+      <c r="B132" t="n">
+        <v>466</v>
+      </c>
+      <c r="C132" t="inlineStr"/>
+      <c r="D132" t="n">
+        <v>1.126332640647888</v>
+      </c>
+      <c r="E132" t="n">
+        <v>-12.16913448393123</v>
+      </c>
+      <c r="F132" t="b">
+        <v>0</v>
+      </c>
+      <c r="G132" t="n">
+        <v>13.06111163112545</v>
+      </c>
+      <c r="H132" t="n">
+        <v>43</v>
+      </c>
+      <c r="I132" t="n">
+        <v>-14.77152493004724</v>
+      </c>
+      <c r="J132" t="n">
+        <v>52</v>
+      </c>
+      <c r="K132" t="b">
+        <v>0</v>
+      </c>
+      <c r="L132" t="inlineStr"/>
+      <c r="M132" t="inlineStr"/>
+      <c r="N132" t="n">
+        <v>25.23024611505668</v>
+      </c>
+      <c r="O132" t="inlineStr"/>
+      <c r="P132" t="inlineStr"/>
+    </row>
+    <row r="133">
+      <c r="A133" t="inlineStr">
+        <is>
+          <t>twelve_bar_breakout</t>
+        </is>
+      </c>
+      <c r="B133" t="n">
+        <v>474</v>
+      </c>
+      <c r="C133" t="inlineStr"/>
+      <c r="D133" t="n">
+        <v>1.180631518363953</v>
+      </c>
+      <c r="E133" t="n">
+        <v>-20.42920155838306</v>
+      </c>
+      <c r="F133" t="b">
+        <v>0</v>
+      </c>
+      <c r="G133" t="n">
+        <v>7.861274612198517</v>
+      </c>
+      <c r="H133" t="n">
+        <v>35</v>
+      </c>
+      <c r="I133" t="n">
+        <v>-20.42920155838306</v>
+      </c>
+      <c r="J133" t="n">
+        <v>52</v>
+      </c>
+      <c r="K133" t="b">
+        <v>1</v>
+      </c>
+      <c r="L133" t="n">
+        <v>52</v>
+      </c>
+      <c r="M133" t="n">
+        <v>-20.42920155838306</v>
+      </c>
+      <c r="N133" t="n">
+        <v>28.29047617058158</v>
+      </c>
+      <c r="O133" t="n">
+        <v>0</v>
+      </c>
+      <c r="P133" t="n">
+        <v>-28.29047617058158</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="inlineStr">
+        <is>
+          <t>twelve_bar_breakout</t>
+        </is>
+      </c>
+      <c r="B134" t="n">
+        <v>570</v>
+      </c>
+      <c r="C134" t="inlineStr"/>
+      <c r="D134" t="n">
+        <v>1.132612466812134</v>
+      </c>
+      <c r="E134" t="n">
+        <v>8.096343537898264</v>
+      </c>
+      <c r="F134" t="b">
+        <v>1</v>
+      </c>
+      <c r="G134" t="n">
+        <v>33.28600500210272</v>
+      </c>
+      <c r="H134" t="n">
+        <v>18</v>
+      </c>
+      <c r="I134" t="n">
+        <v>-3.873702175052806</v>
+      </c>
+      <c r="J134" t="n">
+        <v>1</v>
+      </c>
+      <c r="K134" t="b">
+        <v>1</v>
+      </c>
+      <c r="L134" t="n">
+        <v>36</v>
+      </c>
+      <c r="M134" t="n">
+        <v>16.34909097339008</v>
+      </c>
+      <c r="N134" t="n">
+        <v>25.18966146420446</v>
+      </c>
+      <c r="O134" t="n">
+        <v>8.252747435491813</v>
+      </c>
+      <c r="P134" t="n">
+        <v>-16.93691402871264</v>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="inlineStr">
+        <is>
+          <t>twelve_bar_breakout</t>
+        </is>
+      </c>
+      <c r="B135" t="n">
+        <v>647</v>
+      </c>
+      <c r="C135" t="inlineStr"/>
+      <c r="D135" t="n">
+        <v>1.19927990436554</v>
+      </c>
+      <c r="E135" t="n">
+        <v>32.46787443183789</v>
+      </c>
+      <c r="F135" t="b">
+        <v>1</v>
+      </c>
+      <c r="G135" t="n">
+        <v>41.14286377091877</v>
+      </c>
+      <c r="H135" t="n">
+        <v>51</v>
+      </c>
+      <c r="I135" t="n">
+        <v>-4.452701304248674</v>
+      </c>
+      <c r="J135" t="n">
+        <v>11</v>
+      </c>
+      <c r="K135" t="b">
+        <v>1</v>
+      </c>
+      <c r="L135" t="n">
+        <v>9</v>
+      </c>
+      <c r="M135" t="n">
+        <v>2.040816123671994</v>
+      </c>
+      <c r="N135" t="n">
+        <v>8.674989339080874</v>
+      </c>
+      <c r="O135" t="n">
+        <v>-30.4270583081659</v>
+      </c>
+      <c r="P135" t="n">
+        <v>-39.10204764724677</v>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="inlineStr">
+        <is>
+          <t>twelve_bar_breakout</t>
+        </is>
+      </c>
+      <c r="B136" t="n">
+        <v>675</v>
+      </c>
+      <c r="C136" t="inlineStr"/>
+      <c r="D136" t="n">
+        <v>1.240873217582703</v>
+      </c>
+      <c r="E136" t="n">
+        <v>40.52448223921937</v>
+      </c>
+      <c r="F136" t="b">
+        <v>1</v>
+      </c>
+      <c r="G136" t="n">
+        <v>50.62907998003872</v>
+      </c>
+      <c r="H136" t="n">
+        <v>52</v>
+      </c>
+      <c r="I136" t="n">
+        <v>-2.052262283883473</v>
+      </c>
+      <c r="J136" t="n">
+        <v>0</v>
+      </c>
+      <c r="K136" t="b">
+        <v>1</v>
+      </c>
+      <c r="L136" t="n">
+        <v>10</v>
+      </c>
+      <c r="M136" t="n">
+        <v>7.328527391973195</v>
+      </c>
+      <c r="N136" t="n">
+        <v>10.10459774081935</v>
+      </c>
+      <c r="O136" t="n">
+        <v>-33.19595484724617</v>
+      </c>
+      <c r="P136" t="n">
+        <v>-43.30055258806552</v>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="inlineStr">
+        <is>
+          <t>twelve_bar_breakout</t>
+        </is>
+      </c>
+      <c r="B137" t="n">
+        <v>686</v>
+      </c>
+      <c r="C137" t="inlineStr"/>
+      <c r="D137" t="n">
+        <v>1.351788401603699</v>
+      </c>
+      <c r="E137" t="n">
+        <v>43.67977665571423</v>
+      </c>
+      <c r="F137" t="b">
+        <v>1</v>
+      </c>
+      <c r="G137" t="n">
+        <v>47.54810341828778</v>
+      </c>
+      <c r="H137" t="n">
+        <v>51</v>
+      </c>
+      <c r="I137" t="n">
+        <v>-3.58902819374427</v>
+      </c>
+      <c r="J137" t="n">
+        <v>0</v>
+      </c>
+      <c r="K137" t="b">
+        <v>0</v>
+      </c>
+      <c r="L137" t="inlineStr"/>
+      <c r="M137" t="inlineStr"/>
+      <c r="N137" t="n">
+        <v>3.868326762573552</v>
+      </c>
+      <c r="O137" t="inlineStr"/>
+      <c r="P137" t="inlineStr"/>
+    </row>
+    <row r="138">
+      <c r="A138" t="inlineStr">
+        <is>
+          <t>twelve_bar_breakout</t>
+        </is>
+      </c>
+      <c r="B138" t="n">
+        <v>698</v>
+      </c>
+      <c r="C138" t="inlineStr"/>
+      <c r="D138" t="n">
+        <v>1.593416333198547</v>
+      </c>
+      <c r="E138" t="n">
+        <v>29.312099723601</v>
+      </c>
+      <c r="F138" t="b">
+        <v>1</v>
+      </c>
+      <c r="G138" t="n">
+        <v>44.202595235624</v>
+      </c>
+      <c r="H138" t="n">
+        <v>49</v>
+      </c>
+      <c r="I138" t="n">
+        <v>-13.21849062699777</v>
+      </c>
+      <c r="J138" t="n">
+        <v>14</v>
+      </c>
+      <c r="K138" t="b">
+        <v>0</v>
+      </c>
+      <c r="L138" t="inlineStr"/>
+      <c r="M138" t="inlineStr"/>
+      <c r="N138" t="n">
+        <v>14.89049551202299</v>
+      </c>
+      <c r="O138" t="inlineStr"/>
+      <c r="P138" t="inlineStr"/>
+    </row>
+    <row r="139">
+      <c r="A139" t="inlineStr">
+        <is>
+          <t>twelve_bar_breakout</t>
+        </is>
+      </c>
+      <c r="B139" t="n">
+        <v>726</v>
+      </c>
+      <c r="C139" t="inlineStr"/>
+      <c r="D139" t="n">
+        <v>1.755925059318542</v>
+      </c>
+      <c r="E139" t="n">
+        <v>20.97555921964009</v>
+      </c>
+      <c r="F139" t="b">
+        <v>1</v>
+      </c>
+      <c r="G139" t="n">
+        <v>30.85682063631786</v>
+      </c>
+      <c r="H139" t="n">
+        <v>21</v>
+      </c>
+      <c r="I139" t="n">
+        <v>-3.194449829686965</v>
+      </c>
+      <c r="J139" t="n">
+        <v>0</v>
+      </c>
+      <c r="K139" t="b">
+        <v>1</v>
+      </c>
+      <c r="L139" t="n">
+        <v>30</v>
+      </c>
+      <c r="M139" t="n">
+        <v>15.35312133586363</v>
+      </c>
+      <c r="N139" t="n">
+        <v>9.881261416677766</v>
+      </c>
+      <c r="O139" t="n">
+        <v>-5.622437883776461</v>
+      </c>
+      <c r="P139" t="n">
+        <v>-15.50369930045423</v>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="inlineStr">
+        <is>
+          <t>twelve_bar_breakout</t>
+        </is>
+      </c>
+      <c r="B140" t="n">
+        <v>730</v>
+      </c>
+      <c r="C140" t="inlineStr"/>
+      <c r="D140" t="n">
+        <v>1.848598837852478</v>
+      </c>
+      <c r="E140" t="n">
+        <v>16.97512073607752</v>
+      </c>
+      <c r="F140" t="b">
+        <v>1</v>
+      </c>
+      <c r="G140" t="n">
+        <v>24.86421259070014</v>
+      </c>
+      <c r="H140" t="n">
+        <v>49</v>
+      </c>
+      <c r="I140" t="n">
+        <v>-4.353586542463757</v>
+      </c>
+      <c r="J140" t="n">
+        <v>3</v>
+      </c>
+      <c r="K140" t="b">
+        <v>1</v>
+      </c>
+      <c r="L140" t="n">
+        <v>26</v>
+      </c>
+      <c r="M140" t="n">
+        <v>9.570249789597343</v>
+      </c>
+      <c r="N140" t="n">
+        <v>7.889091854622617</v>
+      </c>
+      <c r="O140" t="n">
+        <v>-7.404870946480182</v>
+      </c>
+      <c r="P140" t="n">
+        <v>-15.2939628011028</v>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" t="inlineStr">
+        <is>
+          <t>twelve_bar_breakout</t>
+        </is>
+      </c>
+      <c r="B141" t="n">
+        <v>778</v>
+      </c>
+      <c r="C141" t="inlineStr"/>
+      <c r="D141" t="n">
+        <v>2.124240159988404</v>
+      </c>
+      <c r="E141" t="n">
+        <v>9.140792364823586</v>
+      </c>
+      <c r="F141" t="b">
+        <v>1</v>
+      </c>
+      <c r="G141" t="n">
+        <v>13.20912879091547</v>
+      </c>
+      <c r="H141" t="n">
+        <v>42</v>
+      </c>
+      <c r="I141" t="n">
+        <v>-8.023919619939516</v>
+      </c>
+      <c r="J141" t="n">
+        <v>8</v>
+      </c>
+      <c r="K141" t="b">
+        <v>1</v>
+      </c>
+      <c r="L141" t="n">
+        <v>23</v>
+      </c>
+      <c r="M141" t="n">
+        <v>0.2561699826559782</v>
+      </c>
+      <c r="N141" t="n">
+        <v>4.06833642609188</v>
+      </c>
+      <c r="O141" t="n">
+        <v>-8.884622382167608</v>
+      </c>
+      <c r="P141" t="n">
+        <v>-12.95295880825949</v>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" t="inlineStr">
+        <is>
+          <t>twelve_bar_breakout</t>
+        </is>
+      </c>
+      <c r="B142" t="n">
+        <v>783</v>
+      </c>
+      <c r="C142" t="inlineStr"/>
+      <c r="D142" t="n">
+        <v>2.106432914733887</v>
+      </c>
+      <c r="E142" t="n">
+        <v>-0.6541354745093956</v>
+      </c>
+      <c r="F142" t="b">
+        <v>0</v>
+      </c>
+      <c r="G142" t="n">
+        <v>14.16616981858319</v>
+      </c>
+      <c r="H142" t="n">
+        <v>37</v>
+      </c>
+      <c r="I142" t="n">
+        <v>-7.246377354329874</v>
+      </c>
+      <c r="J142" t="n">
+        <v>3</v>
+      </c>
+      <c r="K142" t="b">
+        <v>1</v>
+      </c>
+      <c r="L142" t="n">
+        <v>18</v>
+      </c>
+      <c r="M142" t="n">
+        <v>1.103710008579494</v>
+      </c>
+      <c r="N142" t="n">
+        <v>14.82030529309259</v>
+      </c>
+      <c r="O142" t="n">
+        <v>1.757845483088889</v>
+      </c>
+      <c r="P142" t="n">
+        <v>-13.0624598100037</v>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" t="inlineStr">
+        <is>
+          <t>twelve_bar_breakout</t>
+        </is>
+      </c>
+      <c r="B143" t="n">
+        <v>812</v>
+      </c>
+      <c r="C143" t="inlineStr"/>
+      <c r="D143" t="n">
+        <v>2.324469327926636</v>
+      </c>
+      <c r="E143" t="n">
+        <v>-16.734994739747</v>
+      </c>
+      <c r="F143" t="b">
+        <v>0</v>
+      </c>
+      <c r="G143" t="n">
+        <v>3.457324631367259</v>
+      </c>
+      <c r="H143" t="n">
+        <v>8</v>
+      </c>
+      <c r="I143" t="n">
+        <v>-24.18805702641347</v>
+      </c>
+      <c r="J143" t="n">
+        <v>41</v>
+      </c>
+      <c r="K143" t="b">
+        <v>1</v>
+      </c>
+      <c r="L143" t="n">
+        <v>16</v>
+      </c>
+      <c r="M143" t="n">
+        <v>-7.924124760462854</v>
+      </c>
+      <c r="N143" t="n">
+        <v>20.19231937111426</v>
+      </c>
+      <c r="O143" t="n">
+        <v>8.810869979284147</v>
+      </c>
+      <c r="P143" t="n">
+        <v>-11.38144939183011</v>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" t="inlineStr">
+        <is>
+          <t>twelve_bar_breakout</t>
+        </is>
+      </c>
+      <c r="B144" t="n">
+        <v>815</v>
+      </c>
+      <c r="C144" t="inlineStr"/>
+      <c r="D144" t="n">
+        <v>2.338694095611572</v>
+      </c>
+      <c r="E144" t="n">
+        <v>-13.44034994108586</v>
+      </c>
+      <c r="F144" t="b">
+        <v>0</v>
+      </c>
+      <c r="G144" t="n">
+        <v>2.828060457421768</v>
+      </c>
+      <c r="H144" t="n">
+        <v>5</v>
+      </c>
+      <c r="I144" t="n">
+        <v>-24.64917217549024</v>
+      </c>
+      <c r="J144" t="n">
+        <v>38</v>
+      </c>
+      <c r="K144" t="b">
+        <v>1</v>
+      </c>
+      <c r="L144" t="n">
+        <v>13</v>
+      </c>
+      <c r="M144" t="n">
+        <v>-8.484162918992121</v>
+      </c>
+      <c r="N144" t="n">
+        <v>16.26841039850763</v>
+      </c>
+      <c r="O144" t="n">
+        <v>4.956187022093742</v>
+      </c>
+      <c r="P144" t="n">
+        <v>-11.31222337641389</v>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" t="inlineStr">
+        <is>
+          <t>twelve_bar_breakout</t>
+        </is>
+      </c>
+      <c r="B145" t="n">
+        <v>865</v>
+      </c>
+      <c r="C145" t="inlineStr"/>
+      <c r="D145" t="n">
+        <v>1.967954397201538</v>
+      </c>
+      <c r="E145" t="n">
+        <v>-2.886524785748453</v>
+      </c>
+      <c r="F145" t="b">
+        <v>0</v>
+      </c>
+      <c r="G145" t="n">
+        <v>12.13741030474308</v>
+      </c>
+      <c r="H145" t="n">
+        <v>30</v>
+      </c>
+      <c r="I145" t="n">
+        <v>-9.399376081946111</v>
+      </c>
+      <c r="J145" t="n">
+        <v>37</v>
+      </c>
+      <c r="K145" t="b">
+        <v>1</v>
+      </c>
+      <c r="L145" t="n">
+        <v>25</v>
+      </c>
+      <c r="M145" t="n">
+        <v>-0.233584143052524</v>
+      </c>
+      <c r="N145" t="n">
+        <v>15.02393509049153</v>
+      </c>
+      <c r="O145" t="n">
+        <v>2.652940642695929</v>
+      </c>
+      <c r="P145" t="n">
+        <v>-12.3709944477956</v>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" t="inlineStr">
+        <is>
+          <t>twelve_bar_breakout</t>
+        </is>
+      </c>
+      <c r="B146" t="n">
+        <v>930</v>
+      </c>
+      <c r="C146" t="inlineStr"/>
+      <c r="D146" t="n">
+        <v>2.102106809616089</v>
+      </c>
+      <c r="E146" t="n">
+        <v>9.745244205004608</v>
+      </c>
+      <c r="F146" t="b">
+        <v>1</v>
+      </c>
+      <c r="G146" t="n">
+        <v>11.80760958239365</v>
+      </c>
+      <c r="H146" t="n">
+        <v>46</v>
+      </c>
+      <c r="I146" t="n">
+        <v>-11.96118284624354</v>
+      </c>
+      <c r="J146" t="n">
+        <v>38</v>
+      </c>
+      <c r="K146" t="b">
+        <v>0</v>
+      </c>
+      <c r="L146" t="inlineStr"/>
+      <c r="M146" t="inlineStr"/>
+      <c r="N146" t="n">
+        <v>2.062365377389046</v>
+      </c>
+      <c r="O146" t="inlineStr"/>
+      <c r="P146" t="inlineStr"/>
+    </row>
+    <row r="147">
+      <c r="A147" t="inlineStr">
+        <is>
+          <t>twelve_bar_breakout</t>
+        </is>
+      </c>
+      <c r="B147" t="n">
+        <v>934</v>
+      </c>
+      <c r="C147" t="inlineStr"/>
+      <c r="D147" t="n">
+        <v>2.160742044448853</v>
+      </c>
+      <c r="E147" t="n">
+        <v>2.61111097011975</v>
+      </c>
+      <c r="F147" t="b">
+        <v>1</v>
+      </c>
+      <c r="G147" t="n">
+        <v>8.773529016971123</v>
+      </c>
+      <c r="H147" t="n">
+        <v>42</v>
+      </c>
+      <c r="I147" t="n">
+        <v>-14.35025873407169</v>
+      </c>
+      <c r="J147" t="n">
+        <v>34</v>
+      </c>
+      <c r="K147" t="b">
+        <v>1</v>
+      </c>
+      <c r="L147" t="n">
+        <v>52</v>
+      </c>
+      <c r="M147" t="n">
+        <v>2.61111097011975</v>
+      </c>
+      <c r="N147" t="n">
+        <v>6.162418046851373</v>
+      </c>
+      <c r="O147" t="n">
+        <v>0</v>
+      </c>
+      <c r="P147" t="n">
+        <v>-6.162418046851373</v>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" t="inlineStr">
+        <is>
+          <t>twelve_bar_breakout</t>
+        </is>
+      </c>
+      <c r="B148" t="n">
+        <v>987</v>
+      </c>
+      <c r="C148" t="inlineStr"/>
+      <c r="D148" t="n">
+        <v>2.245030641555786</v>
+      </c>
+      <c r="E148" t="n">
+        <v>-1.018081227092329</v>
+      </c>
+      <c r="F148" t="b">
+        <v>0</v>
+      </c>
+      <c r="G148" t="n">
+        <v>12.5950621371932</v>
+      </c>
+      <c r="H148" t="n">
+        <v>14</v>
+      </c>
+      <c r="I148" t="n">
+        <v>-9.087102723460552</v>
+      </c>
+      <c r="J148" t="n">
+        <v>33</v>
+      </c>
+      <c r="K148" t="b">
+        <v>1</v>
+      </c>
+      <c r="L148" t="n">
+        <v>9</v>
+      </c>
+      <c r="M148" t="n">
+        <v>-0.2758290083165198</v>
+      </c>
+      <c r="N148" t="n">
+        <v>13.61314336428553</v>
+      </c>
+      <c r="O148" t="n">
+        <v>0.7422522187758096</v>
+      </c>
+      <c r="P148" t="n">
+        <v>-12.87089114550972</v>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" t="inlineStr">
+        <is>
+          <t>twelve_bar_breakout</t>
+        </is>
+      </c>
+      <c r="B149" t="n">
+        <v>998</v>
+      </c>
+      <c r="C149" t="inlineStr"/>
+      <c r="D149" t="n">
+        <v>2.400268077850342</v>
+      </c>
+      <c r="E149" t="n">
+        <v>-3.931281930863553</v>
+      </c>
+      <c r="F149" t="b">
+        <v>0</v>
+      </c>
+      <c r="G149" t="n">
+        <v>5.312971879484127</v>
+      </c>
+      <c r="H149" t="n">
+        <v>3</v>
+      </c>
+      <c r="I149" t="n">
+        <v>-14.96689808030245</v>
+      </c>
+      <c r="J149" t="n">
+        <v>22</v>
+      </c>
+      <c r="K149" t="b">
+        <v>1</v>
+      </c>
+      <c r="L149" t="n">
+        <v>48</v>
+      </c>
+      <c r="M149" t="n">
+        <v>-7.011882050814436</v>
+      </c>
+      <c r="N149" t="n">
+        <v>9.244253810347681</v>
+      </c>
+      <c r="O149" t="n">
+        <v>-3.080600119950883</v>
+      </c>
+      <c r="P149" t="n">
+        <v>-12.32485393029856</v>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" t="inlineStr">
+        <is>
+          <t>twelve_bar_breakout</t>
+        </is>
+      </c>
+      <c r="B150" t="n">
+        <v>1077</v>
+      </c>
+      <c r="C150" t="inlineStr"/>
+      <c r="D150" t="n">
+        <v>2.062973260879517</v>
+      </c>
+      <c r="E150" t="n">
+        <v>17.46650799625598</v>
+      </c>
+      <c r="F150" t="b">
+        <v>1</v>
+      </c>
+      <c r="G150" t="n">
+        <v>22.45626613256606</v>
+      </c>
+      <c r="H150" t="n">
+        <v>51</v>
+      </c>
+      <c r="I150" t="n">
+        <v>-34.25475020033648</v>
+      </c>
+      <c r="J150" t="n">
+        <v>24</v>
+      </c>
+      <c r="K150" t="b">
+        <v>1</v>
+      </c>
+      <c r="L150" t="n">
+        <v>14</v>
+      </c>
+      <c r="M150" t="n">
+        <v>1.661150685615452</v>
+      </c>
+      <c r="N150" t="n">
+        <v>4.989758136310083</v>
+      </c>
+      <c r="O150" t="n">
+        <v>-15.80535731064053</v>
+      </c>
+      <c r="P150" t="n">
+        <v>-20.79511544695061</v>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" t="inlineStr">
+        <is>
+          <t>twelve_bar_breakout</t>
+        </is>
+      </c>
+      <c r="B151" t="n">
+        <v>1085</v>
+      </c>
+      <c r="C151" t="inlineStr"/>
+      <c r="D151" t="n">
+        <v>2.160053968429565</v>
+      </c>
+      <c r="E151" t="n">
+        <v>10.00300995935619</v>
+      </c>
+      <c r="F151" t="b">
+        <v>1</v>
+      </c>
+      <c r="G151" t="n">
+        <v>16.95263467990859</v>
+      </c>
+      <c r="H151" t="n">
+        <v>43</v>
+      </c>
+      <c r="I151" t="n">
+        <v>-37.20958163598176</v>
+      </c>
+      <c r="J151" t="n">
+        <v>16</v>
+      </c>
+      <c r="K151" t="b">
+        <v>1</v>
+      </c>
+      <c r="L151" t="n">
+        <v>6</v>
+      </c>
+      <c r="M151" t="n">
+        <v>-2.907872395824957</v>
+      </c>
+      <c r="N151" t="n">
+        <v>6.949624720552402</v>
+      </c>
+      <c r="O151" t="n">
+        <v>-12.91088235518115</v>
+      </c>
+      <c r="P151" t="n">
+        <v>-19.86050707573355</v>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" t="inlineStr">
+        <is>
+          <t>twelve_bar_breakout</t>
+        </is>
+      </c>
+      <c r="B152" t="n">
+        <v>1115</v>
+      </c>
+      <c r="C152" t="inlineStr"/>
+      <c r="D152" t="n">
+        <v>1.842256546020508</v>
+      </c>
+      <c r="E152" t="n">
+        <v>50.4313843538436</v>
+      </c>
+      <c r="F152" t="b">
+        <v>1</v>
+      </c>
+      <c r="G152" t="n">
+        <v>61.15940339460346</v>
+      </c>
+      <c r="H152" t="n">
+        <v>47</v>
+      </c>
+      <c r="I152" t="n">
+        <v>-10.03937992494167</v>
+      </c>
+      <c r="J152" t="n">
+        <v>3</v>
+      </c>
+      <c r="K152" t="b">
+        <v>1</v>
+      </c>
+      <c r="L152" t="n">
+        <v>38</v>
+      </c>
+      <c r="M152" t="n">
+        <v>37.59311524392957</v>
+      </c>
+      <c r="N152" t="n">
+        <v>10.72801904075986</v>
+      </c>
+      <c r="O152" t="n">
+        <v>-12.83826910991403</v>
+      </c>
+      <c r="P152" t="n">
+        <v>-23.56628815067389</v>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" t="inlineStr">
+        <is>
+          <t>twelve_bar_breakout</t>
+        </is>
+      </c>
+      <c r="B153" t="n">
+        <v>1139</v>
+      </c>
+      <c r="C153" t="inlineStr"/>
+      <c r="D153" t="n">
+        <v>2.470483541488647</v>
+      </c>
+      <c r="E153" t="n">
+        <v>20.07577910702021</v>
+      </c>
+      <c r="F153" t="b">
+        <v>1</v>
+      </c>
+      <c r="G153" t="n">
+        <v>28.30015461623718</v>
+      </c>
+      <c r="H153" t="n">
+        <v>41</v>
+      </c>
+      <c r="I153" t="n">
+        <v>-3.47223400324099</v>
+      </c>
+      <c r="J153" t="n">
+        <v>0</v>
+      </c>
+      <c r="K153" t="b">
+        <v>1</v>
+      </c>
+      <c r="L153" t="n">
+        <v>14</v>
+      </c>
+      <c r="M153" t="n">
+        <v>2.604131130030528</v>
+      </c>
+      <c r="N153" t="n">
+        <v>8.224375509216966</v>
+      </c>
+      <c r="O153" t="n">
+        <v>-17.47164797698968</v>
+      </c>
+      <c r="P153" t="n">
+        <v>-25.69602348620665</v>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" t="inlineStr">
+        <is>
+          <t>twelve_bar_breakout</t>
+        </is>
+      </c>
+      <c r="B154" t="n">
+        <v>1172</v>
+      </c>
+      <c r="C154" t="inlineStr"/>
+      <c r="D154" t="n">
+        <v>2.995321989059448</v>
+      </c>
+      <c r="E154" t="n">
+        <v>7.948442808496611</v>
+      </c>
+      <c r="F154" t="b">
+        <v>1</v>
+      </c>
+      <c r="G154" t="n">
+        <v>15.07274320705671</v>
+      </c>
+      <c r="H154" t="n">
+        <v>38</v>
+      </c>
+      <c r="I154" t="n">
+        <v>-7.478011942056756</v>
+      </c>
+      <c r="J154" t="n">
+        <v>6</v>
+      </c>
+      <c r="K154" t="b">
+        <v>1</v>
+      </c>
+      <c r="L154" t="n">
+        <v>6</v>
+      </c>
+      <c r="M154" t="n">
+        <v>-2.199423701958334</v>
+      </c>
+      <c r="N154" t="n">
+        <v>7.124300398560099</v>
+      </c>
+      <c r="O154" t="n">
+        <v>-10.14786651045494</v>
+      </c>
+      <c r="P154" t="n">
+        <v>-17.27216690901504</v>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" t="inlineStr">
+        <is>
+          <t>twelve_bar_breakout</t>
+        </is>
+      </c>
+      <c r="B155" t="n">
+        <v>1180</v>
+      </c>
+      <c r="C155" t="inlineStr"/>
+      <c r="D155" t="n">
+        <v>3.079331159591675</v>
+      </c>
+      <c r="E155" t="n">
+        <v>3.5928192856868</v>
+      </c>
+      <c r="F155" t="b">
+        <v>1</v>
+      </c>
+      <c r="G155" t="n">
+        <v>11.93337130885052</v>
+      </c>
+      <c r="H155" t="n">
+        <v>30</v>
+      </c>
+      <c r="I155" t="n">
+        <v>-11.56811972779405</v>
+      </c>
+      <c r="J155" t="n">
+        <v>48</v>
+      </c>
+      <c r="K155" t="b">
+        <v>1</v>
+      </c>
+      <c r="L155" t="n">
+        <v>12</v>
+      </c>
+      <c r="M155" t="n">
+        <v>-4.985354590333866</v>
+      </c>
+      <c r="N155" t="n">
+        <v>8.340552023163717</v>
+      </c>
+      <c r="O155" t="n">
+        <v>-8.578173876020667</v>
+      </c>
+      <c r="P155" t="n">
+        <v>-16.91872589918438</v>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" t="inlineStr">
+        <is>
+          <t>twelve_bar_breakout</t>
+        </is>
+      </c>
+      <c r="B156" t="n">
+        <v>1204</v>
+      </c>
+      <c r="C156" t="inlineStr"/>
+      <c r="D156" t="n">
+        <v>3.201239347457886</v>
+      </c>
+      <c r="E156" t="n">
+        <v>6.071942808247669</v>
+      </c>
+      <c r="F156" t="b">
+        <v>1</v>
+      </c>
+      <c r="G156" t="n">
+        <v>12.64542431452557</v>
+      </c>
+      <c r="H156" t="n">
+        <v>41</v>
+      </c>
+      <c r="I156" t="n">
+        <v>-14.93574367073579</v>
+      </c>
+      <c r="J156" t="n">
+        <v>24</v>
+      </c>
+      <c r="K156" t="b">
+        <v>1</v>
+      </c>
+      <c r="L156" t="n">
+        <v>23</v>
+      </c>
+      <c r="M156" t="n">
+        <v>-6.096021209846956</v>
+      </c>
+      <c r="N156" t="n">
+        <v>6.5734815062779</v>
+      </c>
+      <c r="O156" t="n">
+        <v>-12.16796401809463</v>
+      </c>
+      <c r="P156" t="n">
+        <v>-18.74144552437252</v>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" t="inlineStr">
+        <is>
+          <t>twelve_bar_breakout</t>
+        </is>
+      </c>
+      <c r="B157" t="n">
+        <v>1206</v>
+      </c>
+      <c r="C157" t="inlineStr"/>
+      <c r="D157" t="n">
+        <v>3.187013387680054</v>
+      </c>
+      <c r="E157" t="n">
+        <v>8.2513278856625</v>
+      </c>
+      <c r="F157" t="b">
+        <v>1</v>
+      </c>
+      <c r="G157" t="n">
+        <v>13.14824280962508</v>
+      </c>
+      <c r="H157" t="n">
+        <v>39</v>
+      </c>
+      <c r="I157" t="n">
+        <v>-14.55603999777688</v>
+      </c>
+      <c r="J157" t="n">
+        <v>22</v>
+      </c>
+      <c r="K157" t="b">
+        <v>1</v>
+      </c>
+      <c r="L157" t="n">
+        <v>21</v>
+      </c>
+      <c r="M157" t="n">
+        <v>-5.676859423325707</v>
+      </c>
+      <c r="N157" t="n">
+        <v>4.896914923962578</v>
+      </c>
+      <c r="O157" t="n">
+        <v>-13.92818730898821</v>
+      </c>
+      <c r="P157" t="n">
+        <v>-18.82510223295078</v>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" t="inlineStr">
+        <is>
+          <t>twelve_bar_breakout</t>
+        </is>
+      </c>
+      <c r="B158" t="n">
+        <v>1244</v>
+      </c>
+      <c r="C158" t="inlineStr"/>
+      <c r="D158" t="n">
+        <v>3.548659086227417</v>
+      </c>
+      <c r="E158" t="n">
+        <v>12.73479750781956</v>
+      </c>
+      <c r="F158" t="b">
+        <v>1</v>
+      </c>
+      <c r="G158" t="n">
+        <v>15.44617927398806</v>
+      </c>
+      <c r="H158" t="n">
+        <v>45</v>
+      </c>
+      <c r="I158" t="n">
+        <v>-9.029688320308066</v>
+      </c>
+      <c r="J158" t="n">
+        <v>11</v>
+      </c>
+      <c r="K158" t="b">
+        <v>1</v>
+      </c>
+      <c r="L158" t="n">
+        <v>10</v>
+      </c>
+      <c r="M158" t="n">
+        <v>-6.603834749100638</v>
+      </c>
+      <c r="N158" t="n">
+        <v>2.7113817661685</v>
+      </c>
+      <c r="O158" t="n">
+        <v>-19.33863225692019</v>
+      </c>
+      <c r="P158" t="n">
+        <v>-22.05001402308869</v>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" t="inlineStr">
+        <is>
+          <t>twelve_bar_breakout</t>
+        </is>
+      </c>
+      <c r="B159" t="n">
+        <v>1267</v>
+      </c>
+      <c r="C159" t="inlineStr"/>
+      <c r="D159" t="n">
+        <v>3.804333448410034</v>
+      </c>
+      <c r="E159" t="n">
+        <v>36.94129381881312</v>
+      </c>
+      <c r="F159" t="b">
+        <v>1</v>
+      </c>
+      <c r="G159" t="n">
+        <v>37.75885438673813</v>
+      </c>
+      <c r="H159" t="n">
+        <v>52</v>
+      </c>
+      <c r="I159" t="n">
+        <v>-9.831782980264476</v>
+      </c>
+      <c r="J159" t="n">
+        <v>8</v>
+      </c>
+      <c r="K159" t="b">
+        <v>1</v>
+      </c>
+      <c r="L159" t="n">
+        <v>27</v>
+      </c>
+      <c r="M159" t="n">
+        <v>2.362988546821361</v>
+      </c>
+      <c r="N159" t="n">
+        <v>0.8175605679250069</v>
+      </c>
+      <c r="O159" t="n">
+        <v>-34.57830527199176</v>
+      </c>
+      <c r="P159" t="n">
+        <v>-35.39586583991677</v>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" t="inlineStr">
+        <is>
+          <t>twelve_bar_breakout</t>
+        </is>
+      </c>
+      <c r="B160" t="n">
+        <v>1287</v>
+      </c>
+      <c r="C160" t="inlineStr"/>
+      <c r="D160" t="n">
+        <v>3.929679155349731</v>
+      </c>
+      <c r="E160" t="n">
+        <v>44.0367585312435</v>
+      </c>
+      <c r="F160" t="b">
+        <v>1</v>
+      </c>
+      <c r="G160" t="n">
+        <v>49.5662987029533</v>
+      </c>
+      <c r="H160" t="n">
+        <v>51</v>
+      </c>
+      <c r="I160" t="n">
+        <v>-2.835047030988338</v>
+      </c>
+      <c r="J160" t="n">
+        <v>0</v>
+      </c>
+      <c r="K160" t="b">
+        <v>1</v>
+      </c>
+      <c r="L160" t="n">
+        <v>7</v>
+      </c>
+      <c r="M160" t="n">
+        <v>-0.9021027384032997</v>
+      </c>
+      <c r="N160" t="n">
+        <v>5.529540171709804</v>
+      </c>
+      <c r="O160" t="n">
+        <v>-44.9388612696468</v>
+      </c>
+      <c r="P160" t="n">
+        <v>-50.4684014413566</v>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" t="inlineStr">
+        <is>
+          <t>twelve_bar_breakout</t>
+        </is>
+      </c>
+      <c r="B161" t="n">
+        <v>1306</v>
+      </c>
+      <c r="C161" t="inlineStr"/>
+      <c r="D161" t="n">
+        <v>4.461400985717773</v>
+      </c>
+      <c r="E161" t="n">
+        <v>40.50524163776971</v>
+      </c>
+      <c r="F161" t="b">
+        <v>1</v>
+      </c>
+      <c r="G161" t="n">
+        <v>43.81280385885852</v>
+      </c>
+      <c r="H161" t="n">
+        <v>52</v>
+      </c>
+      <c r="I161" t="n">
+        <v>-4.994328544861387</v>
+      </c>
+      <c r="J161" t="n">
+        <v>0</v>
+      </c>
+      <c r="K161" t="b">
+        <v>1</v>
+      </c>
+      <c r="L161" t="n">
+        <v>35</v>
+      </c>
+      <c r="M161" t="n">
+        <v>22.23721163083103</v>
+      </c>
+      <c r="N161" t="n">
+        <v>3.307562221088801</v>
+      </c>
+      <c r="O161" t="n">
+        <v>-18.26803000693868</v>
+      </c>
+      <c r="P161" t="n">
+        <v>-21.57559222802749</v>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" t="inlineStr">
+        <is>
+          <t>twelve_bar_breakout</t>
+        </is>
+      </c>
+      <c r="B162" t="n">
+        <v>1354</v>
+      </c>
+      <c r="C162" t="inlineStr"/>
+      <c r="D162" t="n">
+        <v>6.12684154510498</v>
+      </c>
+      <c r="E162" t="n">
+        <v>32.84057070019436</v>
+      </c>
+      <c r="F162" t="b">
+        <v>1</v>
+      </c>
+      <c r="G162" t="n">
+        <v>38.05002398159707</v>
+      </c>
+      <c r="H162" t="n">
+        <v>51</v>
+      </c>
+      <c r="I162" t="n">
+        <v>-3.371905165612068</v>
+      </c>
+      <c r="J162" t="n">
+        <v>1</v>
+      </c>
+      <c r="K162" t="b">
+        <v>0</v>
+      </c>
+      <c r="L162" t="inlineStr"/>
+      <c r="M162" t="inlineStr"/>
+      <c r="N162" t="n">
+        <v>5.209453281402709</v>
+      </c>
+      <c r="O162" t="inlineStr"/>
+      <c r="P162" t="inlineStr"/>
+    </row>
+    <row r="163">
+      <c r="A163" t="inlineStr">
+        <is>
+          <t>twelve_bar_breakout</t>
+        </is>
+      </c>
+      <c r="B163" t="n">
+        <v>1374</v>
+      </c>
+      <c r="C163" t="inlineStr"/>
+      <c r="D163" t="n">
+        <v>6.379292964935303</v>
+      </c>
+      <c r="E163" t="n">
+        <v>41.92092640443546</v>
+      </c>
+      <c r="F163" t="b">
+        <v>1</v>
+      </c>
+      <c r="G163" t="n">
+        <v>44.66148064728103</v>
+      </c>
+      <c r="H163" t="n">
+        <v>42</v>
+      </c>
+      <c r="I163" t="n">
+        <v>-6.880300947545541</v>
+      </c>
+      <c r="J163" t="n">
+        <v>6</v>
+      </c>
+      <c r="K163" t="b">
+        <v>1</v>
+      </c>
+      <c r="L163" t="n">
+        <v>48</v>
+      </c>
+      <c r="M163" t="n">
+        <v>32.62264762604827</v>
+      </c>
+      <c r="N163" t="n">
+        <v>2.740554242845569</v>
+      </c>
+      <c r="O163" t="n">
+        <v>-9.298278778387193</v>
+      </c>
+      <c r="P163" t="n">
+        <v>-12.03883302123276</v>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" t="inlineStr">
+        <is>
+          <t>twelve_bar_breakout</t>
+        </is>
+      </c>
+      <c r="B164" t="n">
+        <v>1396</v>
+      </c>
+      <c r="C164" t="inlineStr"/>
+      <c r="D164" t="n">
+        <v>7.193688869476318</v>
+      </c>
+      <c r="E164" t="n">
+        <v>21.04869736095609</v>
+      </c>
+      <c r="F164" t="b">
+        <v>1</v>
+      </c>
+      <c r="G164" t="n">
+        <v>29.58629037762218</v>
+      </c>
+      <c r="H164" t="n">
+        <v>38</v>
+      </c>
+      <c r="I164" t="n">
+        <v>-3.583618316763238</v>
+      </c>
+      <c r="J164" t="n">
+        <v>0</v>
+      </c>
+      <c r="K164" t="b">
+        <v>1</v>
+      </c>
+      <c r="L164" t="n">
+        <v>26</v>
+      </c>
+      <c r="M164" t="n">
+        <v>17.60846741395597</v>
+      </c>
+      <c r="N164" t="n">
+        <v>8.53759301666609</v>
+      </c>
+      <c r="O164" t="n">
+        <v>-3.440229947000116</v>
+      </c>
+      <c r="P164" t="n">
+        <v>-11.97782296366621</v>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" t="inlineStr">
+        <is>
+          <t>twelve_bar_breakout</t>
+        </is>
+      </c>
+      <c r="B165" t="n">
+        <v>1412</v>
+      </c>
+      <c r="C165" t="inlineStr"/>
+      <c r="D165" t="n">
+        <v>8.789555549621582</v>
+      </c>
+      <c r="E165" t="n">
+        <v>0.8850740469528782</v>
+      </c>
+      <c r="F165" t="b">
+        <v>1</v>
+      </c>
+      <c r="G165" t="n">
+        <v>6.058087859329938</v>
+      </c>
+      <c r="H165" t="n">
+        <v>22</v>
+      </c>
+      <c r="I165" t="n">
+        <v>-12.4694675307934</v>
+      </c>
+      <c r="J165" t="n">
+        <v>51</v>
+      </c>
+      <c r="K165" t="b">
+        <v>1</v>
+      </c>
+      <c r="L165" t="n">
+        <v>10</v>
+      </c>
+      <c r="M165" t="n">
+        <v>-3.744993906049324</v>
+      </c>
+      <c r="N165" t="n">
+        <v>5.17301381237706</v>
+      </c>
+      <c r="O165" t="n">
+        <v>-4.630067953002203</v>
+      </c>
+      <c r="P165" t="n">
+        <v>-9.803081765379263</v>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" t="inlineStr">
+        <is>
+          <t>twelve_bar_breakout</t>
+        </is>
+      </c>
+      <c r="B166" t="n">
+        <v>1451</v>
+      </c>
+      <c r="C166" t="inlineStr"/>
+      <c r="D166" t="n">
+        <v>8.803558349609375</v>
+      </c>
+      <c r="E166" t="n">
+        <v>7.289258167952182</v>
+      </c>
+      <c r="F166" t="b">
+        <v>1</v>
+      </c>
+      <c r="G166" t="n">
+        <v>23.01552034532245</v>
+      </c>
+      <c r="H166" t="n">
+        <v>27</v>
+      </c>
+      <c r="I166" t="n">
+        <v>-12.60869220453521</v>
+      </c>
+      <c r="J166" t="n">
+        <v>12</v>
+      </c>
+      <c r="K166" t="b">
+        <v>1</v>
+      </c>
+      <c r="L166" t="n">
+        <v>8</v>
+      </c>
+      <c r="M166" t="n">
+        <v>-8.768123320911689</v>
+      </c>
+      <c r="N166" t="n">
+        <v>15.72626217737027</v>
+      </c>
+      <c r="O166" t="n">
+        <v>-16.05738148886387</v>
+      </c>
+      <c r="P166" t="n">
+        <v>-31.78364366623414</v>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" t="inlineStr">
+        <is>
+          <t>twelve_bar_breakout</t>
+        </is>
+      </c>
+      <c r="B167" t="n">
+        <v>1475</v>
+      </c>
+      <c r="C167" t="inlineStr"/>
+      <c r="D167" t="n">
+        <v>10.41033935546875</v>
+      </c>
+      <c r="E167" t="n">
+        <v>-1.167273969149229</v>
+      </c>
+      <c r="F167" t="b">
+        <v>0</v>
+      </c>
+      <c r="G167" t="n">
+        <v>4.028723203792421</v>
+      </c>
+      <c r="H167" t="n">
+        <v>3</v>
+      </c>
+      <c r="I167" t="n">
+        <v>-13.40302539458242</v>
+      </c>
+      <c r="J167" t="n">
+        <v>28</v>
+      </c>
+      <c r="K167" t="b">
+        <v>1</v>
+      </c>
+      <c r="L167" t="n">
+        <v>28</v>
+      </c>
+      <c r="M167" t="n">
+        <v>-9.270273300774477</v>
+      </c>
+      <c r="N167" t="n">
+        <v>5.195997172941651</v>
+      </c>
+      <c r="O167" t="n">
+        <v>-8.102999331625247</v>
+      </c>
+      <c r="P167" t="n">
+        <v>-13.2989965045669</v>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" t="inlineStr">
+        <is>
+          <t>twelve_bar_breakout</t>
+        </is>
+      </c>
+      <c r="B168" t="n">
+        <v>1516</v>
+      </c>
+      <c r="C168" t="inlineStr"/>
+      <c r="D168" t="n">
+        <v>9.76960277557373</v>
+      </c>
+      <c r="E168" t="n">
+        <v>-2.682364439250361</v>
+      </c>
+      <c r="F168" t="b">
+        <v>0</v>
+      </c>
+      <c r="G168" t="n">
+        <v>15.72885505598791</v>
+      </c>
+      <c r="H168" t="n">
+        <v>18</v>
+      </c>
+      <c r="I168" t="n">
+        <v>-4.203002054347381</v>
+      </c>
+      <c r="J168" t="n">
+        <v>2</v>
+      </c>
+      <c r="K168" t="b">
+        <v>1</v>
+      </c>
+      <c r="L168" t="n">
+        <v>33</v>
+      </c>
+      <c r="M168" t="n">
+        <v>6.873723603403341</v>
+      </c>
+      <c r="N168" t="n">
+        <v>18.41121949523827</v>
+      </c>
+      <c r="O168" t="n">
+        <v>9.556088042653702</v>
+      </c>
+      <c r="P168" t="n">
+        <v>-8.855131452584569</v>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" t="inlineStr">
+        <is>
+          <t>twelve_bar_breakout</t>
+        </is>
+      </c>
+      <c r="B169" t="n">
+        <v>1526</v>
+      </c>
+      <c r="C169" t="inlineStr"/>
+      <c r="D169" t="n">
+        <v>10.58528900146484</v>
+      </c>
+      <c r="E169" t="n">
+        <v>-9.303399798909497</v>
+      </c>
+      <c r="F169" t="b">
+        <v>0</v>
+      </c>
+      <c r="G169" t="n">
+        <v>6.810965993700131</v>
+      </c>
+      <c r="H169" t="n">
+        <v>8</v>
+      </c>
+      <c r="I169" t="n">
+        <v>-11.08942771318078</v>
+      </c>
+      <c r="J169" t="n">
+        <v>42</v>
+      </c>
+      <c r="K169" t="b">
+        <v>1</v>
+      </c>
+      <c r="L169" t="n">
+        <v>23</v>
+      </c>
+      <c r="M169" t="n">
+        <v>-1.361802534893527</v>
+      </c>
+      <c r="N169" t="n">
+        <v>16.11436579260963</v>
+      </c>
+      <c r="O169" t="n">
+        <v>7.941597264015971</v>
+      </c>
+      <c r="P169" t="n">
+        <v>-8.172768528593657</v>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" t="inlineStr">
+        <is>
+          <t>twelve_bar_breakout</t>
+        </is>
+      </c>
+      <c r="B170" t="n">
+        <v>1591</v>
+      </c>
+      <c r="C170" t="inlineStr"/>
+      <c r="D170" t="n">
+        <v>10.41161060333252</v>
+      </c>
+      <c r="E170" t="n">
+        <v>11.33441082165887</v>
+      </c>
+      <c r="F170" t="b">
+        <v>1</v>
+      </c>
+      <c r="G170" t="n">
+        <v>18.63382615790207</v>
+      </c>
+      <c r="H170" t="n">
+        <v>49</v>
+      </c>
+      <c r="I170" t="n">
+        <v>-12.95835301447059</v>
+      </c>
+      <c r="J170" t="n">
+        <v>13</v>
+      </c>
+      <c r="K170" t="b">
+        <v>0</v>
+      </c>
+      <c r="L170" t="inlineStr"/>
+      <c r="M170" t="inlineStr"/>
+      <c r="N170" t="n">
+        <v>7.299415336243198</v>
+      </c>
+      <c r="O170" t="inlineStr"/>
+      <c r="P170" t="inlineStr"/>
+    </row>
+    <row r="171">
+      <c r="A171" t="inlineStr">
+        <is>
+          <t>twelve_bar_breakout</t>
+        </is>
+      </c>
+      <c r="B171" t="n">
+        <v>1618</v>
+      </c>
+      <c r="C171" t="inlineStr"/>
+      <c r="D171" t="n">
+        <v>9.867429733276367</v>
+      </c>
+      <c r="E171" t="n">
+        <v>21.65910068378961</v>
+      </c>
+      <c r="F171" t="b">
+        <v>1</v>
+      </c>
+      <c r="G171" t="n">
+        <v>25.17638693428995</v>
+      </c>
+      <c r="H171" t="n">
+        <v>22</v>
+      </c>
+      <c r="I171" t="n">
+        <v>-2.683102875870939</v>
+      </c>
+      <c r="J171" t="n">
+        <v>0</v>
+      </c>
+      <c r="K171" t="b">
+        <v>0</v>
+      </c>
+      <c r="L171" t="inlineStr"/>
+      <c r="M171" t="inlineStr"/>
+      <c r="N171" t="n">
+        <v>3.517286250500337</v>
+      </c>
+      <c r="O171" t="inlineStr"/>
+      <c r="P171" t="inlineStr"/>
+    </row>
+    <row r="172">
+      <c r="A172" t="inlineStr">
+        <is>
+          <t>twelve_bar_breakout</t>
+        </is>
+      </c>
+      <c r="B172" t="n">
+        <v>1669</v>
+      </c>
+      <c r="C172" t="inlineStr"/>
+      <c r="D172" t="n">
+        <v>11.7477617263794</v>
+      </c>
+      <c r="E172" t="n">
+        <v>-2.464390525376603</v>
+      </c>
+      <c r="F172" t="b">
+        <v>0</v>
+      </c>
+      <c r="G172" t="n">
+        <v>9.85495573471232</v>
+      </c>
+      <c r="H172" t="n">
+        <v>43</v>
+      </c>
+      <c r="I172" t="n">
+        <v>-35.76184248416661</v>
+      </c>
+      <c r="J172" t="n">
+        <v>8</v>
+      </c>
+      <c r="K172" t="b">
+        <v>1</v>
+      </c>
+      <c r="L172" t="n">
+        <v>50</v>
+      </c>
+      <c r="M172" t="n">
+        <v>0.4953313415737292</v>
+      </c>
+      <c r="N172" t="n">
+        <v>12.31934626008892</v>
+      </c>
+      <c r="O172" t="n">
+        <v>2.959721866950332</v>
+      </c>
+      <c r="P172" t="n">
+        <v>-9.35962439313859</v>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" t="inlineStr">
+        <is>
+          <t>twelve_bar_breakout</t>
+        </is>
+      </c>
+      <c r="B173" t="n">
+        <v>1692</v>
+      </c>
+      <c r="C173" t="inlineStr"/>
+      <c r="D173" t="n">
+        <v>11.79929447174072</v>
+      </c>
+      <c r="E173" t="n">
+        <v>5.190238284925929</v>
+      </c>
+      <c r="F173" t="b">
+        <v>1</v>
+      </c>
+      <c r="G173" t="n">
+        <v>9.375170483643682</v>
+      </c>
+      <c r="H173" t="n">
+        <v>20</v>
+      </c>
+      <c r="I173" t="n">
+        <v>-8.000001751008586</v>
+      </c>
+      <c r="J173" t="n">
+        <v>0</v>
+      </c>
+      <c r="K173" t="b">
+        <v>1</v>
+      </c>
+      <c r="L173" t="n">
+        <v>27</v>
+      </c>
+      <c r="M173" t="n">
+        <v>0.0564237160007911</v>
+      </c>
+      <c r="N173" t="n">
+        <v>4.184932198717753</v>
+      </c>
+      <c r="O173" t="n">
+        <v>-5.133814568925138</v>
+      </c>
+      <c r="P173" t="n">
+        <v>-9.318746767642891</v>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" t="inlineStr">
+        <is>
+          <t>twelve_bar_breakout</t>
+        </is>
+      </c>
+      <c r="B174" t="n">
+        <v>1736</v>
+      </c>
+      <c r="C174" t="inlineStr"/>
+      <c r="D174" t="n">
+        <v>12.817551612854</v>
+      </c>
+      <c r="E174" t="n">
+        <v>15.41183572210396</v>
+      </c>
+      <c r="F174" t="b">
+        <v>1</v>
+      </c>
+      <c r="G174" t="n">
+        <v>17.3558943314939</v>
+      </c>
+      <c r="H174" t="n">
+        <v>52</v>
+      </c>
+      <c r="I174" t="n">
+        <v>-6.04359678596194</v>
+      </c>
+      <c r="J174" t="n">
+        <v>3</v>
+      </c>
+      <c r="K174" t="b">
+        <v>1</v>
+      </c>
+      <c r="L174" t="n">
+        <v>20</v>
+      </c>
+      <c r="M174" t="n">
+        <v>2.587168308869728</v>
+      </c>
+      <c r="N174" t="n">
+        <v>1.944058609389938</v>
+      </c>
+      <c r="O174" t="n">
+        <v>-12.82466741323423</v>
+      </c>
+      <c r="P174" t="n">
+        <v>-14.76872602262417</v>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" t="inlineStr">
+        <is>
+          <t>twelve_bar_breakout</t>
+        </is>
+      </c>
+      <c r="B175" t="n">
+        <v>1772</v>
+      </c>
+      <c r="C175" t="inlineStr"/>
+      <c r="D175" t="n">
+        <v>13.91074085235596</v>
+      </c>
+      <c r="E175" t="n">
+        <v>7.368273980495238</v>
+      </c>
+      <c r="F175" t="b">
+        <v>1</v>
+      </c>
+      <c r="G175" t="n">
+        <v>14.66835886464928</v>
+      </c>
+      <c r="H175" t="n">
+        <v>31</v>
+      </c>
+      <c r="I175" t="n">
+        <v>-12.64543962705433</v>
+      </c>
+      <c r="J175" t="n">
+        <v>8</v>
+      </c>
+      <c r="K175" t="b">
+        <v>1</v>
+      </c>
+      <c r="L175" t="n">
+        <v>6</v>
+      </c>
+      <c r="M175" t="n">
+        <v>-7.092209910431362</v>
+      </c>
+      <c r="N175" t="n">
+        <v>7.300084884154045</v>
+      </c>
+      <c r="O175" t="n">
+        <v>-14.4604838909266</v>
+      </c>
+      <c r="P175" t="n">
+        <v>-21.76056877508065</v>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" t="inlineStr">
+        <is>
+          <t>twelve_bar_breakout</t>
+        </is>
+      </c>
+      <c r="B176" t="n">
+        <v>1803</v>
+      </c>
+      <c r="C176" t="inlineStr"/>
+      <c r="D176" t="n">
+        <v>15.2722635269165</v>
+      </c>
+      <c r="E176" t="n">
+        <v>-14.27041707981745</v>
+      </c>
+      <c r="F176" t="b">
+        <v>0</v>
+      </c>
+      <c r="G176" t="n">
+        <v>4.445671810192221</v>
+      </c>
+      <c r="H176" t="n">
+        <v>0</v>
+      </c>
+      <c r="I176" t="n">
+        <v>-19.42794326485621</v>
+      </c>
+      <c r="J176" t="n">
+        <v>52</v>
+      </c>
+      <c r="K176" t="b">
+        <v>1</v>
+      </c>
+      <c r="L176" t="n">
+        <v>5</v>
+      </c>
+      <c r="M176" t="n">
+        <v>-7.045659492314568</v>
+      </c>
+      <c r="N176" t="n">
+        <v>18.71608889000968</v>
+      </c>
+      <c r="O176" t="n">
+        <v>7.224757587502886</v>
+      </c>
+      <c r="P176" t="n">
+        <v>-11.49133130250679</v>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" t="inlineStr">
+        <is>
+          <t>twelve_bar_breakout</t>
+        </is>
+      </c>
+      <c r="B177" t="n">
+        <v>1880</v>
+      </c>
+      <c r="C177" t="inlineStr"/>
+      <c r="D177" t="n">
+        <v>12.58901405334473</v>
+      </c>
+      <c r="E177" t="n">
+        <v>20.41378162011274</v>
+      </c>
+      <c r="F177" t="b">
+        <v>1</v>
+      </c>
+      <c r="G177" t="n">
+        <v>25.6857067168388</v>
+      </c>
+      <c r="H177" t="n">
+        <v>36</v>
+      </c>
+      <c r="I177" t="n">
+        <v>-2.498228742212191</v>
+      </c>
+      <c r="J177" t="n">
+        <v>3</v>
+      </c>
+      <c r="K177" t="b">
+        <v>1</v>
+      </c>
+      <c r="L177" t="n">
+        <v>3</v>
+      </c>
+      <c r="M177" t="n">
+        <v>0.2141200608641718</v>
+      </c>
+      <c r="N177" t="n">
+        <v>5.271925096726061</v>
+      </c>
+      <c r="O177" t="n">
+        <v>-20.19966155924857</v>
+      </c>
+      <c r="P177" t="n">
+        <v>-25.47158665597463</v>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" t="inlineStr">
+        <is>
+          <t>twelve_bar_breakout</t>
+        </is>
+      </c>
+      <c r="B178" t="n">
+        <v>1904</v>
+      </c>
+      <c r="C178" t="inlineStr"/>
+      <c r="D178" t="n">
+        <v>14.45338821411133</v>
+      </c>
+      <c r="E178" t="n">
+        <v>-0.2901657460313232</v>
+      </c>
+      <c r="F178" t="b">
+        <v>0</v>
+      </c>
+      <c r="G178" t="n">
+        <v>9.47323248524072</v>
+      </c>
+      <c r="H178" t="n">
+        <v>12</v>
+      </c>
+      <c r="I178" t="n">
+        <v>-7.268513289917689</v>
+      </c>
+      <c r="J178" t="n">
+        <v>45</v>
+      </c>
+      <c r="K178" t="b">
+        <v>1</v>
+      </c>
+      <c r="L178" t="n">
+        <v>17</v>
+      </c>
+      <c r="M178" t="n">
+        <v>3.663929790129971</v>
+      </c>
+      <c r="N178" t="n">
+        <v>9.763398231272044</v>
+      </c>
+      <c r="O178" t="n">
+        <v>3.954095536161294</v>
+      </c>
+      <c r="P178" t="n">
+        <v>-5.809302695110749</v>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" t="inlineStr">
+        <is>
+          <t>twelve_bar_breakout</t>
+        </is>
+      </c>
+      <c r="B179" t="n">
+        <v>1916</v>
+      </c>
+      <c r="C179" t="inlineStr"/>
+      <c r="D179" t="n">
+        <v>15.62667560577393</v>
+      </c>
+      <c r="E179" t="n">
+        <v>-20.77427365729883</v>
+      </c>
+      <c r="F179" t="b">
+        <v>0</v>
+      </c>
+      <c r="G179" t="n">
+        <v>1.253725877448695</v>
+      </c>
+      <c r="H179" t="n">
+        <v>0</v>
+      </c>
+      <c r="I179" t="n">
+        <v>-24.24078754164876</v>
+      </c>
+      <c r="J179" t="n">
+        <v>51</v>
+      </c>
+      <c r="K179" t="b">
+        <v>1</v>
+      </c>
+      <c r="L179" t="n">
+        <v>5</v>
+      </c>
+      <c r="M179" t="n">
+        <v>-4.119400769827124</v>
+      </c>
+      <c r="N179" t="n">
+        <v>22.02799953474753</v>
+      </c>
+      <c r="O179" t="n">
+        <v>16.65487288747171</v>
+      </c>
+      <c r="P179" t="n">
+        <v>-5.373126647275819</v>
       </c>
     </row>
   </sheetData>
@@ -6625,7 +9187,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T4"/>
+  <dimension ref="A1:T5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6838,40 +9400,90 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
+          <t>twelve_bar_breakout</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>53</v>
+      </c>
+      <c r="C4" t="n">
+        <v>66.0377358490566</v>
+      </c>
+      <c r="D4" t="n">
+        <v>10.78554124932222</v>
+      </c>
+      <c r="E4" t="n">
+        <v>7.948442808496611</v>
+      </c>
+      <c r="F4" t="n">
+        <v>19.42903125416979</v>
+      </c>
+      <c r="G4" t="n">
+        <v>21.18535398584186</v>
+      </c>
+      <c r="H4" t="n">
+        <v>-11.26447868764851</v>
+      </c>
+      <c r="I4" t="n">
+        <v>10.39981273651965</v>
+      </c>
+      <c r="J4" t="n">
+        <v>79.24528301886792</v>
+      </c>
+      <c r="K4" t="n">
+        <v>21.80952380952381</v>
+      </c>
+      <c r="L4" t="n">
+        <v>28.57142857142857</v>
+      </c>
+      <c r="M4" t="n">
+        <v>-7.916058245813068</v>
+      </c>
+      <c r="N4" t="inlineStr"/>
+      <c r="O4" t="inlineStr"/>
+      <c r="P4" t="inlineStr"/>
+      <c r="Q4" t="inlineStr"/>
+      <c r="R4" t="inlineStr"/>
+      <c r="S4" t="inlineStr"/>
+      <c r="T4" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
           <t>random_baseline</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr"/>
-      <c r="C4" t="inlineStr"/>
-      <c r="D4" t="inlineStr"/>
-      <c r="E4" t="inlineStr"/>
-      <c r="F4" t="inlineStr"/>
-      <c r="G4" t="inlineStr"/>
-      <c r="H4" t="inlineStr"/>
-      <c r="I4" t="inlineStr"/>
-      <c r="J4" t="inlineStr"/>
-      <c r="K4" t="inlineStr"/>
-      <c r="L4" t="inlineStr"/>
-      <c r="M4" t="inlineStr"/>
-      <c r="N4" t="n">
+      <c r="B5" t="inlineStr"/>
+      <c r="C5" t="inlineStr"/>
+      <c r="D5" t="inlineStr"/>
+      <c r="E5" t="inlineStr"/>
+      <c r="F5" t="inlineStr"/>
+      <c r="G5" t="inlineStr"/>
+      <c r="H5" t="inlineStr"/>
+      <c r="I5" t="inlineStr"/>
+      <c r="J5" t="inlineStr"/>
+      <c r="K5" t="inlineStr"/>
+      <c r="L5" t="inlineStr"/>
+      <c r="M5" t="inlineStr"/>
+      <c r="N5" t="n">
         <v>500</v>
       </c>
-      <c r="O4" t="n">
+      <c r="O5" t="n">
         <v>71.39999999999999</v>
       </c>
-      <c r="P4" t="n">
+      <c r="P5" t="n">
         <v>10.90021021336762</v>
       </c>
-      <c r="Q4" t="n">
+      <c r="Q5" t="n">
         <v>9.418466482550292</v>
       </c>
-      <c r="R4" t="n">
+      <c r="R5" t="n">
         <v>18.20430199089318</v>
       </c>
-      <c r="S4" t="n">
+      <c r="S5" t="n">
         <v>21.24088605902904</v>
       </c>
-      <c r="T4" t="n">
+      <c r="T5" t="n">
         <v>-10.48600020622952</v>
       </c>
     </row>

</xml_diff>